<commit_message>
create form macro for date picker and test on Company, rename php_setting, change loan acc # (sub_branch-client_id)
</commit_message>
<xml_diff>
--- a/app/storage/packages/loan/Repayment Schedule.xlsx
+++ b/app/storage/packages/loan/Repayment Schedule.xlsx
@@ -198,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -230,27 +230,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -275,17 +275,20 @@
     <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,135 +594,148 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F6" sqref="F6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="12" t="s">
         <v>27</v>
       </c>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="2" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="E6" s="12"/>
+      <c r="F6" s="12" t="s">
         <v>28</v>
       </c>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12" t="s">
         <v>29</v>
       </c>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="E8" s="12"/>
+      <c r="F8" s="12" t="s">
         <v>30</v>
       </c>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
         <v>31</v>
       </c>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -745,107 +761,137 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="9">
         <v>0</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="9">
         <v>0</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="10">
         <v>0</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="10">
         <v>0</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="10">
         <f>D13+E13</f>
         <v>0</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="10">
         <v>4000000</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="9">
         <v>1</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="9">
         <v>0</v>
       </c>
-      <c r="D14" s="13">
-        <v>10000</v>
-      </c>
-      <c r="E14" s="13">
+      <c r="D14" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="E14" s="10">
         <v>2000</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="10">
         <f>D14+E14</f>
-        <v>12000</v>
-      </c>
-      <c r="G14" s="13">
+        <v>10002000</v>
+      </c>
+      <c r="G14" s="10">
         <v>4000000</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="F21" s="10" t="s">
+    <row r="20" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="F21" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+    <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="4" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="22">
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.25" footer="0.25"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
fix Repayment Schedule report
</commit_message>
<xml_diff>
--- a/app/storage/packages/loan/Repayment Schedule.xlsx
+++ b/app/storage/packages/loan/Repayment Schedule.xlsx
@@ -60,9 +60,6 @@
     <t>អាសយដ្ឋាន៖ ទូរស័ព្ទ៖</t>
   </si>
   <si>
-    <t>*ធ្វើការពីថ្ងៃច័ន្ទ ដល់ សុក្រ ម៉ោង ០៧-៣០ នាទីព្រឹក ដល់ ម៉ោង ០៤-៣០ នាទីល្ងាច ។</t>
-  </si>
-  <si>
     <t>ព្រហស្បតិ៍-28-04-2014</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>*សូមមកបង់ប្រាក់ឲបានមុនម៉ោង ០៣:០០ រសៀល បើសិនថ្ងៃសងប្រាក់ចំថ្ងៃឈប់សម្រាក ត្រូវមកបង់ប្រាក់ឲបានមុន ។</t>
+  </si>
+  <si>
+    <t>*ធ្វើការពីថ្ងៃច័ន្ទ ដល់ សុក្រ និងម៉ោង ០៧-៣០ នាទីព្រឹក ដល់ ម៉ោង ០៤-៣០ នាទីល្ងាច ។</t>
   </si>
 </sst>
 </file>
@@ -172,16 +172,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Khmer OS Muol Light"/>
-    </font>
-    <font>
       <b/>
       <u/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Khmer OS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Khmer OS Muol Light"/>
     </font>
   </fonts>
   <fills count="3">
@@ -198,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -224,15 +224,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -243,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -266,29 +257,35 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,23 +588,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:G6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
@@ -630,105 +628,105 @@
       <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="11"/>
+      <c r="A5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="17"/>
       <c r="F5" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -760,57 +758,68 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
         <v>0</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="9">
+      <c r="B13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="8">
         <v>0</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>0</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <v>0</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="9">
         <f>D13+E13</f>
         <v>0</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="9">
         <v>4000000</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <v>1</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="9">
+      <c r="B14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="8">
         <v>0</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>10000000</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <v>2000</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="9">
         <f>D14+E14</f>
         <v>10002000</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="9">
         <v>4000000</v>
       </c>
+    </row>
+    <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
@@ -819,78 +828,67 @@
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+    <row r="17" spans="2:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="F21" s="7" t="s">
+    <row r="18" spans="2:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="2:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="F19" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>32</v>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A17:G17"/>
     <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A15:G15"/>
     <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.25" footer="0.25"/>
+  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.25" footer="0.25"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;P of &amp;N</oddFooter>

</xml_diff>

<commit_message>
update repayment schedule report form.
</commit_message>
<xml_diff>
--- a/app/storage/packages/loan/Repayment Schedule.xlsx
+++ b/app/storage/packages/loan/Repayment Schedule.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>កាលវិភាគសងប្រាក់</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t xml:space="preserve">ចំនួនទឹកប្រាក់៖ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">សោហ៊ុយសេវា៖ </t>
   </si>
   <si>
     <t xml:space="preserve">មន្រ្តីឥណទាន៖ </t>
@@ -257,35 +254,35 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,7 +588,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:G6"/>
+      <selection activeCell="F8" sqref="F8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -606,227 +603,223 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="8"/>
+      <c r="G5" s="17"/>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="17"/>
+      <c r="F6" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="17"/>
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8" t="s">
+      <c r="E7" s="17"/>
+      <c r="F7" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8" t="s">
+      <c r="E8" s="17"/>
+      <c r="F8" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="8"/>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="8"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
     </row>
     <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="A13" s="9">
         <v>0</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="9">
         <v>0</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="11">
         <v>0</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="11">
         <v>0</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="11">
         <f>D13+E13</f>
         <v>0</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="11">
         <v>4000000</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14" s="9">
         <v>1</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="9">
         <v>0</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="11">
         <v>10000000</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="11">
         <v>2000</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="11">
         <f>D14+E14</f>
         <v>10002000</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="11">
         <v>4000000</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
     </row>
     <row r="17" spans="2:6" ht="21" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
@@ -856,24 +849,17 @@
     </row>
     <row r="21" spans="2:6" ht="21" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
+  <mergeCells count="21">
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F8:G8"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="A16:G16"/>
     <mergeCell ref="A15:G15"/>
@@ -882,10 +868,16 @@
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
create new repayment schedule format for Nikom.
</commit_message>
<xml_diff>
--- a/app/storage/packages/loan/Repayment Schedule.xlsx
+++ b/app/storage/packages/loan/Repayment Schedule.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>កាលវិភាគសងប្រាក់</t>
   </si>
@@ -54,12 +54,6 @@
     <t>ក្រុមហ៊ុន</t>
   </si>
   <si>
-    <t>សាខា</t>
-  </si>
-  <si>
-    <t>អាសយដ្ឋាន៖ ទូរស័ព្ទ៖</t>
-  </si>
-  <si>
     <t>ព្រហស្បតិ៍-28-04-2014</t>
   </si>
   <si>
@@ -111,10 +105,13 @@
     <t xml:space="preserve">ថ្ងៃទី </t>
   </si>
   <si>
-    <t>*ធ្វើការពីថ្ងៃច័ន្ទ ដល់ សុក្រ និងម៉ោង ០៧-៣០ នាទីព្រឹក ដល់ ម៉ោង ០៤-៣០ នាទីល្ងាច ។</t>
-  </si>
-  <si>
-    <t>*សូមមកបង់ប្រាក់ឱ្យបានមុនម៉ោង ០៣:០០ រសៀល បើសិនថ្ងៃសងប្រាក់ចំថ្ងៃឈប់សម្រាក ត្រូវមកបង់ប្រាក់ឱ្យបានមុន ។</t>
+    <t>សាខា, អាសយដ្ឋាន៖, ទូរស័ព្ទ៖</t>
+  </si>
+  <si>
+    <t>*ករណីសងត្រឡប់មានការយីតយ៉ាវ ខ្ញុំបាទ/នាងខ្ញុំ សុខចិត្តលក់ទ្រព្យសម្បត្តិ ដើម្បីសងមកឱ្យស្ថាប័នគ្រប់ចំនួន។</t>
+  </si>
+  <si>
+    <t>*ក្រោយពីបានពិនិត្យកិច្ចសន្យាខ្ចីប្រាក់ NK02 ខ្ញុំបាទ/នាងខ្ញុំ យល់ព្រមសងប្រាក់ តាមពេលវេលាដែលបានកំណត់ក្នុងតារាងនេះ។</t>
   </si>
 </sst>
 </file>
@@ -231,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -260,19 +257,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -585,16 +579,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:G8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="13.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" style="1" customWidth="1"/>
@@ -615,7 +609,7 @@
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -624,9 +618,9 @@
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -635,255 +629,237 @@
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="D4" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-    </row>
-    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="F4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="16"/>
+    </row>
+    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="17"/>
-    </row>
-    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="E7" s="16"/>
+      <c r="F7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="E8" s="16"/>
+      <c r="F8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17" t="s">
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>0</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
+        <f>D10+E10</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="10">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>1</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="E11" s="10">
+        <v>2000</v>
+      </c>
+      <c r="F11" s="10">
+        <f>D11+E11</f>
+        <v>10002000</v>
+      </c>
+      <c r="G11" s="10">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="F16" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="17"/>
-    </row>
-    <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-    </row>
-    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
-        <v>0</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="9">
-        <v>0</v>
-      </c>
-      <c r="D13" s="11">
-        <v>0</v>
-      </c>
-      <c r="E13" s="11">
-        <v>0</v>
-      </c>
-      <c r="F13" s="11">
-        <f>D13+E13</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="11">
-        <v>4000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>1</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="9">
-        <v>0</v>
-      </c>
-      <c r="D14" s="11">
-        <v>10000000</v>
-      </c>
-      <c r="E14" s="11">
-        <v>2000</v>
-      </c>
-      <c r="F14" s="11">
-        <f>D14+E14</f>
-        <v>10002000</v>
-      </c>
-      <c r="G14" s="11">
-        <v>4000000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-    </row>
-    <row r="17" spans="2:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="2:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="F19" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>30</v>
+      <c r="F18" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="D9:E9"/>
+  <mergeCells count="20">
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A8:C8"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A9:C9"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.25" footer="0.25"/>
+  <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;P of &amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;"Khmer OS,Regular"&amp;7-ធ្វើការពីថ្ងៃច័ន្ទ ដល់ សុក្រ និងម៉ោង ០៧-៣០ នាទីព្រឹក ដល់ ម៉ោង ០៤-៣០ នាទីល្ងាច ។
+-សូមមកបង់ប្រាក់ឱ្យបានមុនម៉ោង ០៣:០០ រសៀល បើសិនថ្ងៃសងប្រាក់ចំថ្ងៃឈប់សម្រាក ត្រូវមកបង់ប្រាក់ឱ្យបានមុន ។</oddFooter>
   </headerFooter>
 </worksheet>
 </file>

</xml_diff>